<commit_message>
Update the requirements table.
Change-Id: I00361c71b5002d44cbb46f67b1b16753c4e14a57
Signed-off-by: jeremie.tatibouet <jeremie.tatibouet@cea.fr>
</commit_message>
<xml_diff>
--- a/Documents/PSSM-Requirements.xlsx
+++ b/Documents/PSSM-Requirements.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="304">
   <si>
     <t>id : String [1]</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Deferred_001</t>
   </si>
   <si>
-    <t>A State may specify a set of Event types that may be deferred in that State. This means that Event occurrences of those types will not be dispatched as long as that State remains active. Instead, these Event occurrences remain in the event pool until a state configuration is reached where these Event types are no longer deferred or, if a deferred Event type is used explicitly in a Trigger of a Transition whose source is the deferring State (i.e., a kind of override option). (p.323)</t>
-  </si>
-  <si>
     <t>Deferred_002</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>a Transition terminating on this Pseudostate implies restoring the Region to that same state configuration, but with all the semantics of entering a State (see the Subclause describing State entry). The entry Behaviors of all States in the restored state configuration are performed in the appropriate order starting with the outermost State. (p.326)</t>
   </si>
   <si>
-    <t>History_006</t>
-  </si>
-  <si>
     <t>represents the most recent active substate of its containing Region, but not the substates of that substate. A Transition terminating on this Pseudostate implies restoring the Region to that substate with all the semantics of entering a State. A single outgoing Transition from this Pseudostate may be defined terminating on a substate of the composite State. This substate is the default shallow history state of the composite State. (p.326)</t>
   </si>
   <si>
@@ -557,9 +551,6 @@
     <t>Event_004</t>
   </si>
   <si>
-    <t>it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. In those cases, only one is selected and executed. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. (p.330) The set of Transitions that will fire are the Transitions in the Regions of the current state configuration that satisfy the following conditions: All Transitions in the set are enabled. There are no conflicting Transitions within the set. There is no Transition outside the set that has higher priority than a Transition in the set (that is, enabled Transitions with highest priorities are in the set while conflicting Transitions with lower priorities are left out).</t>
-  </si>
-  <si>
     <t>Event_005</t>
   </si>
   <si>
@@ -596,12 +587,6 @@
     <t>When all orthogonal Regions have finished executing the Transition, the current Event occurrence is fully consumed, and the run-to-completion step is completed. (p.330)</t>
   </si>
   <si>
-    <t>Event_012</t>
-  </si>
-  <si>
-    <t>it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. In those cases, only one is selected and executed. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. (p.330) The set of Transitions that will fire are the Transitions in the Regions of the current state configuration that satisfy the following conditions: All Transitions in the set are enabled. There are no conflicting Transitions within the set. There is no Transition outside the set that has higher priority than a Transition in the set (that is, enabled Transitions with highest priorities are in the set while conflicting Transitions with lower priorities are left out). (p.331-332)</t>
-  </si>
-  <si>
     <t>Event_013</t>
   </si>
   <si>
@@ -671,10 +656,137 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Related to Transition_007. The test for requirement Transition_007 also verifies requirement Transition_009</t>
-  </si>
-  <si>
     <t>Outside the scope of PSSM</t>
+  </si>
+  <si>
+    <t>As fUML is agnostic of time and PSSM relies ont it, the duration of a transition traversal is considered as being "zero" time.</t>
+  </si>
+  <si>
+    <t>There is no dedicated test for requirement "Transition003" but typically test "Entering011" shows the case of transition executed as part of a more complex compound transitions.</t>
+  </si>
+  <si>
+    <t>Cannot be tested by the test suite</t>
+  </si>
+  <si>
+    <t>Exit001 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Cannot be tested by the test suite. Information that is materialized within the runtime</t>
+  </si>
+  <si>
+    <t>Junction_001</t>
+  </si>
+  <si>
+    <t>Junction_002</t>
+  </si>
+  <si>
+    <t>Junction_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is actually shown in test Fork_001 and Fork_002 as well as in other tests located in the "Entering" section </t>
+  </si>
+  <si>
+    <t>NEUTRAL</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Deferred_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if a deferred Event type is used explicitly in a Trigger of a Transition whose source is the deferring State (i.e., a kind of override option)</t>
+  </si>
+  <si>
+    <t>A State may specify a set of Event types that may be deferred in that State. This means that Event occurrences of those types will not be dispatched as long as that State remains active. Instead, these Event occurrences remain in the event pool until a state configuration is reached where these Event types are no longer deferred. (p.323)</t>
+  </si>
+  <si>
+    <t>Behavior 001  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Behavior 002  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Behavior 003 - A and B Tests verifies this requirement</t>
+  </si>
+  <si>
+    <t>Behavior 004  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Choice 001  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Choice 002  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Choice 003  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Deferred 001  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Deferred 003  Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Deferred 002 Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Entry002-C test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Entry002-D test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Behavior003-A and Behavior003-B show support for this requirement</t>
+  </si>
+  <si>
+    <t>Entering 004 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Entering 005 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Entering 009 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Entering 010 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Same as Entering_006</t>
+  </si>
+  <si>
+    <t>Entering 011 test verifies this requirement. Note that is is something that is also shwown in Transition 017 test.</t>
+  </si>
+  <si>
+    <t>Fork 001 Test shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Behavior003-A and B Tests shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Entry 002 tests shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Event 001 test shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Event 002 test shows support for this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is something that can be observed in several existing tests of the PSSM test suite. As an example "Exiting001", "Entering011" demonstrates execution of a step that leads to fire a number of transition. This is considered as being verified even though there is not test dedicated to requirement "Event003" </t>
+  </si>
+  <si>
+    <t>it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. In those cases, only one is selected and executed. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. The set of Transitions that will fire are the Transitions in the Regions of the current state configuration that satisfy the following conditions: All Transitions in the set are enabled. There are no conflicting Transitions within the set. There is no Transition outside the set that has higher priority than a Transition in the set (that is, enabled Transitions with highest priorities are in the set while conflicting Transitions with lower priorities are left out).</t>
+  </si>
+  <si>
+    <t>Event 015 and Event 016 shows support for this requirement</t>
+  </si>
+  <si>
+    <t>For instance a state-machine cannot receive call events.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This does not need to be tested since it ensure by fUML semantics that PSSM does not change. Nevertheless such one by on e disptaching can be observed in all presented tests.
+</t>
   </si>
   <si>
     <r>
@@ -683,7 +795,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
@@ -700,116 +812,155 @@
     </r>
   </si>
   <si>
-    <t>If such transitions do not have triggers they are considered as anonymous transitions.</t>
-  </si>
-  <si>
-    <t>This is also something that is demonstrated by the execution of the test Transitions017 showing how completion events are handled in the context of a composite containing orthogonal regions</t>
-  </si>
-  <si>
-    <t>As fUML is agnostic of time and PSSM relies ont it, the duration of a transition traversal is considered as being "zero" time.</t>
-  </si>
-  <si>
-    <t>There is no dedicated test for requirement "Transition003" but typically test "Entering011" shows the case of transition executed as part of a more complex compound transitions.</t>
-  </si>
-  <si>
-    <t>Cannot be tested by the test suite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is something that is ensured by fUML common behavior event dispatching mechanism  </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>In those cases, only one is selected and executed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. (p.330)</t>
-    </r>
-  </si>
-  <si>
-    <t>Entry002-ter test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Entry002-quater test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Exit001 test verifies this requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is something that can be observed in several existing tests of the PSSM test suite. As an example "Exiting001", "Event008", "Entering011" demonstrates execution of a step that leads to fire a number of transition. This is considered as being verified even though there is not test dedicated to requirement "Event003" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overlap with Event_012. See tests Event_015 and Event_017 </t>
-  </si>
-  <si>
-    <t>Cannot be tested by the test suite. Information that is materialized within the runtime</t>
-  </si>
-  <si>
-    <t>See test Exiting_003</t>
-  </si>
-  <si>
-    <t>See tests Choice_001, Choice_002 and Choice_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The case of the choice pseudo state is supported. See test Choice_002 </t>
-  </si>
-  <si>
-    <t>Overlap with Event_004. See tests Event_015</t>
-  </si>
-  <si>
-    <t>This is tested by "Fork001"</t>
-  </si>
-  <si>
-    <t>Junction_001</t>
-  </si>
-  <si>
-    <t>Junction_002</t>
-  </si>
-  <si>
-    <t>Junction_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is actually shown in test Fork_001 and Fork_002 as well as in other tests located in the "Entering" section </t>
-  </si>
-  <si>
-    <t>There is no dedicated test case for "Region_002" nevertheless a number of test cases cover the default activation of a region. Please see "Entering009" and "Entering011"</t>
-  </si>
-  <si>
-    <t>NEUTRAL</t>
-  </si>
-  <si>
-    <t>This can be observed in test "Event_009"</t>
-  </si>
-  <si>
-    <t>See test Transition011-quinquies</t>
-  </si>
-  <si>
-    <t>See test Final001</t>
-  </si>
-  <si>
-    <t>Coverage</t>
+    <t>Event 008 test verifies this requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event 009 test verifies this requirement but Event 016 -B test highlights some limitations </t>
+  </si>
+  <si>
+    <t>it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. In those cases, only one is selected and executed. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. (p.330)</t>
+  </si>
+  <si>
+    <t>Event 010 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Event_009 shows support of this requirement</t>
+  </si>
+  <si>
+    <t>Event 015 test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Call events need to be supported in fUML first.</t>
+  </si>
+  <si>
+    <t>Any receive event are not supported. This is also the case for call event. Hence the requirement cannot be considered as being supported;</t>
+  </si>
+  <si>
+    <t>Event 016 - A test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>There is no test to demonstrate such support for transitions chained in a compound transition.</t>
+  </si>
+  <si>
+    <t>TransitionSelectionAlgorithmTest and Event 018  shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Exit 001 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exit 002 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exiting 001 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exiting 002 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exiting 003 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exiting 004 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Exiting 005 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Final 001 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Deep history is not supported</t>
+  </si>
+  <si>
+    <t>History pseudostates not supported</t>
+  </si>
+  <si>
+    <t>Join 001 and Join 002 tests verify this requirement.</t>
+  </si>
+  <si>
+    <t>Junction pseudostate is not supported</t>
+  </si>
+  <si>
+    <t>Entering 011 and Entry002-D tests show support for this requirement.</t>
+  </si>
+  <si>
+    <t>Final 001  and Entering 011 show support for this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terminate 001 and Terminate 003 tests verify this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terminate 002 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Transition 001 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Transition 007 test verifies this requirement.</t>
+  </si>
+  <si>
+    <t>Transition 007 and Event 016 A tests show support for this requirement.</t>
+  </si>
+  <si>
+    <t>Transition 007 test show support for this requirement.</t>
+  </si>
+  <si>
+    <t>Transition 010 and Transition 011 - C test show support for this requirement.</t>
+  </si>
+  <si>
+    <t>Transition 011 - A, B, D and E tests show support for this requirement.</t>
+  </si>
+  <si>
+    <t>Behavior 004 test shows support for this requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exiting 003 test shows support for this requirement</t>
+  </si>
+  <si>
+    <t>Transition 011 - A shows support for this requirement</t>
+  </si>
+  <si>
+    <t>Transition 015 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition 016 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition 017 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition 020 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition 019 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition 022 verifies this requirement</t>
+  </si>
+  <si>
+    <t>Transition017  and Final001 shows support of this requirement.</t>
+  </si>
+  <si>
+    <t>This is currently not supported by the execution model.</t>
+  </si>
+  <si>
+    <t>Choice_001, Choice_002 and Choice_003 show support for this requirement.</t>
+  </si>
+  <si>
+    <t>A number of tests use this. Tests such as Transition 007 and Transition 017 shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Entering 011 and Transition 017 shows support for this requirement.</t>
+  </si>
+  <si>
+    <t>Choice case is tested while the join case remain not tested</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -977,14 +1128,8 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1194,8 +1339,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1364,6 +1521,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1410,7 +1580,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1457,9 +1627,6 @@
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1469,12 +1636,8 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="12" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="12" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1491,10 +1654,31 @@
     <xf numFmtId="0" fontId="20" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="12" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="14" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1545,19 +1729,19 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1764,13 +1948,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>108</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2768,10 +2952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,46 +2972,46 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G3" s="2">
-        <f xml:space="preserve"> ROWS(C7:C114)</f>
-        <v>108</v>
+        <f xml:space="preserve"> ROWS(C7:C113)</f>
+        <v>107</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G4" s="2">
-        <f xml:space="preserve"> COUNTIF(C7:C114,"YES") + COUNTIF(C7:C114,"NEUTRAL")</f>
-        <v>85</v>
+        <f xml:space="preserve"> COUNTIF(C7:C113,"YES") + COUNTIF(C7:C113,"NEUTRAL")</f>
+        <v>88</v>
       </c>
       <c r="H4" s="4">
         <f xml:space="preserve"> (G4 * 100) / G3</f>
-        <v>78.703703703703709</v>
+        <v>82.242990654205613</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F5" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G5" s="2">
-        <f xml:space="preserve"> COUNTIF(D7:D114,"YES") + COUNTIF(D7:D114,"NEUTRAL")</f>
-        <v>83</v>
+        <f xml:space="preserve"> COUNTIF(D7:D113,"YES") + COUNTIF(D7:D113,"NEUTRAL")</f>
+        <v>87</v>
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> (G5 * 100) / G3</f>
-        <v>76.851851851851848</v>
+        <v>81.308411214953267</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2838,13 +3022,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -2855,12 +3039,14 @@
         <v>21</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -2870,12 +3056,14 @@
         <v>23</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E8" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -2885,12 +3073,14 @@
         <v>25</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -2900,90 +3090,98 @@
         <v>27</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E11" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="C14" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="B15" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>89</v>
-      </c>
       <c r="C15" s="15" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -2991,767 +3189,825 @@
         <v>35</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="B17" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C18" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="B22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C22" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C23" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E22" s="22"/>
-    </row>
-    <row r="23" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="B24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C24" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="30"/>
+    </row>
+    <row r="25" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="B25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C25" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E24" s="18"/>
-    </row>
-    <row r="25" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="B26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C26" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="B27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="30"/>
+    </row>
+    <row r="28" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E26" s="18"/>
-    </row>
-    <row r="27" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C28" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="B29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E28" s="18"/>
-    </row>
-    <row r="29" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="B30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C30" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E29" s="18"/>
-    </row>
-    <row r="30" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C31" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E30" s="18"/>
-    </row>
-    <row r="31" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C32" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="B33" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C33" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="B34" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="C34" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" s="22"/>
-    </row>
-    <row r="36" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="C36" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="C37" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="C39" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E38" s="18"/>
-    </row>
-    <row r="39" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="C40" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B41" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="B42" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="C42" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="B43" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="C43" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E41" s="18"/>
-    </row>
-    <row r="42" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="B44" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C44" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="B45" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B46" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="C46" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="B47" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B48" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="C48" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="B49" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>194</v>
-      </c>
       <c r="C49" s="15" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>217</v>
+        <v>203</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E50" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E51" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E52" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E53" s="22"/>
+        <v>203</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E54" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C55" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E55" s="18"/>
-    </row>
-    <row r="56" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>214</v>
+      <c r="B56" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E57" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="C58" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E58" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="C59" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E59" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="C60" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E60" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C61" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="C62" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E62" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="C63" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="C64" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E64" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
@@ -3761,821 +4017,858 @@
         <v>29</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E65" s="18"/>
-    </row>
-    <row r="66" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>29</v>
+      <c r="B66" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E66" s="18"/>
-    </row>
-    <row r="67" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>32</v>
+      <c r="B67" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E67" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
+      <c r="A68" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>34</v>
+      <c r="B68" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E68" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="7" t="s">
+      <c r="A69" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E69" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E69" s="31" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="70" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E70" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="C71" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E71" s="18"/>
-    </row>
-    <row r="72" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="C72" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" s="31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C72" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E72" s="18"/>
-    </row>
-    <row r="73" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="C73" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E73" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>100</v>
+      <c r="A74" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E74" s="18"/>
-    </row>
-    <row r="75" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>5</v>
+        <v>202</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E75" s="18"/>
-    </row>
-    <row r="76" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>7</v>
+        <v>202</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E76" s="25" t="s">
-        <v>241</v>
+        <v>202</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>9</v>
+      <c r="A77" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E77" s="25" t="s">
-        <v>240</v>
+        <v>221</v>
+      </c>
+      <c r="E77" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>11</v>
+      <c r="A78" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E78" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>13</v>
+      <c r="A79" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>15</v>
+      <c r="A80" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>17</v>
+      <c r="A81" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E81" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>19</v>
+      <c r="A82" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B83" s="21" t="s">
+      <c r="A83" s="19" t="s">
         <v>81</v>
       </c>
+      <c r="B83" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="C83" s="15" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E83" s="19" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="E83" s="33" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B84" s="21" t="s">
+      <c r="A84" s="19" t="s">
         <v>83</v>
       </c>
+      <c r="B84" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="C84" s="15" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="E84" s="33" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85" s="21" t="s">
-        <v>85</v>
+      <c r="A85" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>217</v>
+        <v>202</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="7" t="s">
         <v>115</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E86" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="8" t="s">
         <v>117</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E87" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="7" t="s">
         <v>119</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E88" s="18"/>
-    </row>
-    <row r="89" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E88" s="34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="8" t="s">
         <v>121</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E89" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="15" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E90" s="25" t="s">
-        <v>222</v>
+      <c r="E90" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E91" s="25" t="s">
-        <v>231</v>
+        <v>221</v>
+      </c>
+      <c r="E91" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
+      <c r="A92" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E92" s="25" t="s">
-        <v>231</v>
+        <v>221</v>
+      </c>
+      <c r="E92" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B93" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E93" s="25" t="s">
-        <v>231</v>
+        <v>202</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="7" t="s">
         <v>131</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E94" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B95" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E95" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="7" t="s">
         <v>135</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E96" s="23" t="s">
-        <v>216</v>
+        <v>202</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B97" s="23" t="s">
         <v>137</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D97" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E97" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="27" t="s">
+      <c r="A98" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B98" s="26" t="s">
+      <c r="B98" s="7" t="s">
         <v>139</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E98" s="30"/>
+        <v>202</v>
+      </c>
+      <c r="E98" s="21" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="99" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E99" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="26" t="s">
         <v>143</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E100" s="25" t="s">
-        <v>232</v>
+        <v>202</v>
+      </c>
+      <c r="E100" s="35" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="8" t="s">
         <v>145</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E101" s="31" t="s">
-        <v>244</v>
+        <v>202</v>
+      </c>
+      <c r="E101" s="22" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
+      <c r="A102" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="7" t="s">
         <v>147</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E102" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="8" t="s">
         <v>149</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E103" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="20" t="s">
         <v>151</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E104" s="22"/>
+        <v>221</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E105" s="22" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B105" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D105" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E105" s="19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
+      <c r="B106" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E106" s="22" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="D106" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E106" s="22"/>
-    </row>
-    <row r="107" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D107" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E107" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="E107" s="27" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="108" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
+      <c r="A108" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="7" t="s">
         <v>159</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E108" s="31" t="s">
-        <v>245</v>
+        <v>202</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B109" s="8" t="s">
         <v>161</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E109" s="18"/>
+        <v>203</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="110" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="7" t="s">
         <v>163</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E110" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B111" s="8" t="s">
         <v>165</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E111" s="24" t="s">
-        <v>233</v>
+        <v>202</v>
+      </c>
+      <c r="E111" s="22" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" s="7" t="s">
         <v>167</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D112" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E112" s="25" t="s">
-        <v>219</v>
+        <v>202</v>
+      </c>
+      <c r="E112" s="22" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B113" s="8" t="s">
         <v>169</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E113" s="18"/>
-    </row>
-    <row r="114" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D114" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E114" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
+      </c>
+      <c r="E113" s="22" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:G108">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="C7:C114">
+  <conditionalFormatting sqref="C7:C113">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D114">
+  <conditionalFormatting sqref="D7:D113">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D114">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="C7:D113">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"NEUTRAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"YES"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NEUTRAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C115:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C114:C1048576">
       <formula1>"OK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D113">
       <formula1>"YES,NO,NEUTRAL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update of requirement coverage: 95% of coverage.
Change-Id: I52f2dc115581d17aad0f36bef7faa0431f344d78
Signed-off-by: jeremie.tatibouet <jeremie.tatibouet@cea.fr>
</commit_message>
<xml_diff>
--- a/Documents/PSSM-Requirements.xlsx
+++ b/Documents/PSSM-Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JT605650\Documents\2015\projets\PSSM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\JT605650\repositories\github\PSSM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="312">
   <si>
     <t>id : String [1]</t>
   </si>
@@ -737,9 +737,6 @@
     <t>Entry002-D test verifies this requirement</t>
   </si>
   <si>
-    <t>Behavior003-A and Behavior003-B show support for this requirement</t>
-  </si>
-  <si>
     <t>Entering 004 test verifies this requirement</t>
   </si>
   <si>
@@ -752,9 +749,6 @@
     <t>Entering 010 test verifies this requirement</t>
   </si>
   <si>
-    <t>Same as Entering_006</t>
-  </si>
-  <si>
     <t>Entering 011 test verifies this requirement. Note that is is something that is also shwown in Transition 017 test.</t>
   </si>
   <si>
@@ -780,9 +774,6 @@
   </si>
   <si>
     <t>Event 015 and Event 016 shows support for this requirement</t>
-  </si>
-  <si>
-    <t>For instance a state-machine cannot receive call events.</t>
   </si>
   <si>
     <t xml:space="preserve">This does not need to be tested since it ensure by fUML semantics that PSSM does not change. Nevertheless such one by on e disptaching can be observed in all presented tests.
@@ -830,9 +821,6 @@
     <t>Event 015 test verifies this requirement</t>
   </si>
   <si>
-    <t>Call events need to be supported in fUML first.</t>
-  </si>
-  <si>
     <t>Any receive event are not supported. This is also the case for call event. Hence the requirement cannot be considered as being supported;</t>
   </si>
   <si>
@@ -869,18 +857,12 @@
     <t>Final 001 test verifies this requirement.</t>
   </si>
   <si>
-    <t>Deep history is not supported</t>
-  </si>
-  <si>
     <t>History pseudostates not supported</t>
   </si>
   <si>
     <t>Join 001 and Join 002 tests verify this requirement.</t>
   </si>
   <si>
-    <t>Junction pseudostate is not supported</t>
-  </si>
-  <si>
     <t>Entering 011 and Entry002-D tests show support for this requirement.</t>
   </si>
   <si>
@@ -954,6 +936,49 @@
   </si>
   <si>
     <t>Choice case is tested while the join case remain not tested</t>
+  </si>
+  <si>
+    <t>History001_Test_A verifies this requirement</t>
+  </si>
+  <si>
+    <t>History_002_Test_A verifies  this requirement</t>
+  </si>
+  <si>
+    <t>Behavior003-A and Behavior003-B verifies this requirement</t>
+  </si>
+  <si>
+    <t>Duplication of Entering001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This does not need to be tested since it ensure by fUML semantics that PSSM does not change. Nevertheless such one by on e disptaching can be observed in all presented tests cases.
+</t>
+  </si>
+  <si>
+    <t>State-machines can respond to signal, event, call event and completion event which event type supported in PSSM context. Support for this requirement is demonstrated by Event017-X and Event019-X test series.</t>
+  </si>
+  <si>
+    <t>Event_019_X serie verifies this requirement</t>
+  </si>
+  <si>
+    <t>History001_Test_A and History001_Test_B verify this requirement</t>
+  </si>
+  <si>
+    <t>History001_Test_B (deep history)verify this requirement. Note: Add an additional test for shallow history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History001_Test_A and History001_Test_B verify this requirement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">History002_Test_A and History002_Test_B verify this requirement </t>
+  </si>
+  <si>
+    <t>Junction00X test serie verifies this requirement</t>
+  </si>
+  <si>
+    <t>Junction003_Test and Junction004_Test verifies this requirement</t>
+  </si>
+  <si>
+    <t>Junction003_Test verifies this requirement</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1889,7 @@
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1951,10 +1976,10 @@
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,12 +1995,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="231248640"/>
-        <c:axId val="231400112"/>
-        <c:axId val="0"/>
+        <c:axId val="16250144"/>
+        <c:axId val="212236320"/>
+        <c:axId val="369399648"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="231248640"/>
+        <c:axId val="16250144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2037,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231400112"/>
+        <c:crossAx val="212236320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,9 +2045,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231400112"/>
+        <c:axId val="212236320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2040,7 +2066,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2071,10 +2097,50 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231248640"/>
+        <c:crossAx val="16250144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:serAx>
+        <c:axId val="369399648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="212236320"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2658,16 +2724,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>261937</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>321467</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>345280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>8020050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>583406</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2954,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,11 +3060,11 @@
       </c>
       <c r="G4" s="2">
         <f xml:space="preserve"> COUNTIF(C7:C113,"YES") + COUNTIF(C7:C113,"NEUTRAL")</f>
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H4" s="4">
         <f xml:space="preserve"> (G4 * 100) / G3</f>
-        <v>82.242990654205613</v>
+        <v>95.327102803738313</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3007,11 +3073,11 @@
       </c>
       <c r="G5" s="2">
         <f xml:space="preserve"> COUNTIF(D7:D113,"YES") + COUNTIF(D7:D113,"NEUTRAL")</f>
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> (G5 * 100) / G3</f>
-        <v>81.308411214953267</v>
+        <v>94.392523364485982</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3294,12 +3360,14 @@
         <v>39</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E22" s="30"/>
+        <v>202</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -3315,7 +3383,7 @@
         <v>202</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>238</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3326,12 +3394,14 @@
         <v>43</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" s="30"/>
+        <v>202</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
@@ -3347,7 +3417,7 @@
         <v>202</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3364,7 +3434,7 @@
         <v>202</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3375,12 +3445,14 @@
         <v>39</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E27" s="30"/>
+        <v>202</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -3405,13 +3477,13 @@
         <v>39</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>243</v>
+        <v>202</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3428,7 +3500,7 @@
         <v>202</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,7 +3517,7 @@
         <v>202</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -3462,7 +3534,7 @@
         <v>202</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3479,7 +3551,7 @@
         <v>202</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3513,7 +3585,7 @@
         <v>202</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3530,7 +3602,7 @@
         <v>202</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3564,7 +3636,7 @@
         <v>202</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3581,10 +3653,10 @@
         <v>202</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>173</v>
       </c>
@@ -3598,7 +3670,7 @@
         <v>202</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3606,7 +3678,7 @@
         <v>175</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>202</v>
@@ -3615,10 +3687,10 @@
         <v>202</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>176</v>
       </c>
@@ -3626,16 +3698,16 @@
         <v>177</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>178</v>
       </c>
@@ -3649,10 +3721,10 @@
         <v>221</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>180</v>
       </c>
@@ -3666,7 +3738,7 @@
         <v>221</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>254</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3674,7 +3746,7 @@
         <v>182</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>202</v>
@@ -3683,7 +3755,7 @@
         <v>202</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3700,7 +3772,7 @@
         <v>202</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3708,7 +3780,7 @@
         <v>185</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>202</v>
@@ -3717,7 +3789,7 @@
         <v>202</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3734,7 +3806,7 @@
         <v>202</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3745,13 +3817,13 @@
         <v>189</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>262</v>
+        <v>202</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
@@ -3768,7 +3840,7 @@
         <v>203</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3785,7 +3857,7 @@
         <v>202</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3802,7 +3874,7 @@
         <v>202</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3819,7 +3891,7 @@
         <v>203</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.25">
@@ -3836,7 +3908,7 @@
         <v>202</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3853,7 +3925,7 @@
         <v>202</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3887,7 +3959,7 @@
         <v>202</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3904,7 +3976,7 @@
         <v>202</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3921,7 +3993,7 @@
         <v>202</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3938,7 +4010,7 @@
         <v>202</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3955,7 +4027,7 @@
         <v>202</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3972,7 +4044,7 @@
         <v>202</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,7 +4078,7 @@
         <v>202</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4017,13 +4089,13 @@
         <v>29</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E65" s="31" t="s">
-        <v>275</v>
+        <v>202</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4034,13 +4106,13 @@
         <v>32</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>275</v>
+        <v>202</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4057,7 +4129,7 @@
         <v>203</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4068,13 +4140,13 @@
         <v>92</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>276</v>
+        <v>202</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4085,13 +4157,13 @@
         <v>93</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>276</v>
+        <v>202</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4108,7 +4180,7 @@
         <v>202</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4119,13 +4191,13 @@
         <v>96</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>278</v>
+        <v>202</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4136,13 +4208,13 @@
         <v>97</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E72" s="31" t="s">
-        <v>278</v>
+        <v>202</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4153,13 +4225,13 @@
         <v>98</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E73" s="31" t="s">
-        <v>278</v>
+        <v>202</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4176,7 +4248,7 @@
         <v>202</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4193,7 +4265,7 @@
         <v>202</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4363,7 +4435,7 @@
         <v>202</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4380,7 +4452,7 @@
         <v>202</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4397,7 +4469,7 @@
         <v>202</v>
       </c>
       <c r="E87" s="22" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4408,10 +4480,10 @@
         <v>119</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="E88" s="34" t="s">
         <v>212</v>
@@ -4499,7 +4571,7 @@
         <v>202</v>
       </c>
       <c r="E93" s="22" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4516,7 +4588,7 @@
         <v>202</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4533,7 +4605,7 @@
         <v>202</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4550,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4567,7 +4639,7 @@
         <v>202</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4584,7 +4656,7 @@
         <v>202</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4601,7 +4673,7 @@
         <v>202</v>
       </c>
       <c r="E99" s="22" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4618,7 +4690,7 @@
         <v>202</v>
       </c>
       <c r="E100" s="35" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4635,7 +4707,7 @@
         <v>202</v>
       </c>
       <c r="E101" s="22" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4652,7 +4724,7 @@
         <v>202</v>
       </c>
       <c r="E102" s="22" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4669,7 +4741,7 @@
         <v>202</v>
       </c>
       <c r="E103" s="22" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4703,7 +4775,7 @@
         <v>202</v>
       </c>
       <c r="E105" s="22" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4720,7 +4792,7 @@
         <v>202</v>
       </c>
       <c r="E106" s="22" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4737,7 +4809,7 @@
         <v>202</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4754,7 +4826,7 @@
         <v>202</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4771,7 +4843,7 @@
         <v>203</v>
       </c>
       <c r="E109" s="31" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4788,7 +4860,7 @@
         <v>202</v>
       </c>
       <c r="E110" s="22" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4805,7 +4877,7 @@
         <v>202</v>
       </c>
       <c r="E111" s="22" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4822,7 +4894,7 @@
         <v>202</v>
       </c>
       <c r="E112" s="22" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4839,7 +4911,7 @@
         <v>203</v>
       </c>
       <c r="E113" s="22" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Requirements covered at 99%.
Change-Id: I2ce2c77855278e38c6d3aad6373ed5f71f9f668e
Signed-off-by: jeremie.tatibouet <jeremie.tatibouet@cea.fr>
</commit_message>
<xml_diff>
--- a/Documents/PSSM-Requirements.xlsx
+++ b/Documents/PSSM-Requirements.xlsx
@@ -818,9 +818,6 @@
     <t>Event 015 test verifies this requirement</t>
   </si>
   <si>
-    <t>Any receive event are not supported. This is also the case for call event. Hence the requirement cannot be considered as being supported;</t>
-  </si>
-  <si>
     <t>Event 016 - A test verifies this requirement.</t>
   </si>
   <si>
@@ -915,9 +912,6 @@
   </si>
   <si>
     <t>Transition017  and Final001 shows support of this requirement.</t>
-  </si>
-  <si>
-    <t>This is currently not supported by the execution model.</t>
   </si>
   <si>
     <t>Choice_001, Choice_002 and Choice_003 show support for this requirement.</t>
@@ -1019,6 +1013,12 @@
   </si>
   <si>
     <t>History_002_Test_C verifies  this requirement</t>
+  </si>
+  <si>
+    <t>Tests Transition_023_Test, Entry002_Test_E and All the Junction_00X serie verify this requirement.</t>
+  </si>
+  <si>
+    <t>See all Event_00X_Test serie as well as Transition_023_Test and Junction_00X serie.</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2020,10 @@
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3064,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,11 +3104,11 @@
       </c>
       <c r="G4" s="2">
         <f xml:space="preserve"> COUNTIF(C7:C113,"YES") + COUNTIF(C7:C113,"NEUTRAL")</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H4" s="4">
         <f xml:space="preserve"> (G4 * 100) / G3</f>
-        <v>97.196261682242991</v>
+        <v>99.065420560747668</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3117,11 +3117,11 @@
       </c>
       <c r="G5" s="2">
         <f xml:space="preserve"> COUNTIF(D7:D113,"YES") + COUNTIF(D7:D113,"NEUTRAL")</f>
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> (G5 * 100) / G3</f>
-        <v>96.261682242990659</v>
+        <v>99.065420560747668</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
         <v>201</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
         <v>201</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3444,7 +3444,7 @@
         <v>201</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
         <v>201</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3503,7 +3503,7 @@
         <v>49</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>201</v>
@@ -3512,7 +3512,7 @@
         <v>201</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3529,7 +3529,7 @@
         <v>201</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3750,7 +3750,7 @@
         <v>201</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3784,7 +3784,7 @@
         <v>220</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3869,7 +3869,7 @@
         <v>201</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
@@ -3880,13 +3880,13 @@
         <v>190</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>258</v>
+        <v>201</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3920,7 +3920,7 @@
         <v>201</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3937,7 +3937,7 @@
         <v>202</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.25">
@@ -3954,7 +3954,7 @@
         <v>201</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3971,7 +3971,7 @@
         <v>201</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>201</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
         <v>201</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4039,7 +4039,7 @@
         <v>201</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4056,7 +4056,7 @@
         <v>201</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>201</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
         <v>201</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
         <v>201</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
         <v>201</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4158,7 +4158,7 @@
         <v>201</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4175,7 +4175,7 @@
         <v>201</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4192,7 +4192,7 @@
         <v>201</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>201</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4226,7 +4226,7 @@
         <v>201</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4243,7 +4243,7 @@
         <v>201</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4260,7 +4260,7 @@
         <v>201</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4277,7 +4277,7 @@
         <v>201</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>201</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>201</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4481,7 +4481,7 @@
         <v>201</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4498,7 +4498,7 @@
         <v>201</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
         <v>201</v>
       </c>
       <c r="E87" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4617,7 +4617,7 @@
         <v>201</v>
       </c>
       <c r="E93" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>201</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4651,7 +4651,7 @@
         <v>201</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4668,7 +4668,7 @@
         <v>201</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4685,7 +4685,7 @@
         <v>201</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>201</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4719,7 +4719,7 @@
         <v>201</v>
       </c>
       <c r="E99" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4736,7 +4736,7 @@
         <v>201</v>
       </c>
       <c r="E100" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4753,7 +4753,7 @@
         <v>201</v>
       </c>
       <c r="E101" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4770,7 +4770,7 @@
         <v>201</v>
       </c>
       <c r="E102" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
         <v>201</v>
       </c>
       <c r="E103" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4821,7 +4821,7 @@
         <v>201</v>
       </c>
       <c r="E105" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4838,7 +4838,7 @@
         <v>201</v>
       </c>
       <c r="E106" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4855,7 +4855,7 @@
         <v>201</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4872,7 +4872,7 @@
         <v>201</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4883,13 +4883,13 @@
         <v>160</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="E109" s="30" t="s">
-        <v>291</v>
+        <v>201</v>
+      </c>
+      <c r="E109" s="22" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4906,7 +4906,7 @@
         <v>201</v>
       </c>
       <c r="E110" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4923,7 +4923,7 @@
         <v>201</v>
       </c>
       <c r="E111" s="22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4940,7 +4940,7 @@
         <v>201</v>
       </c>
       <c r="E112" s="22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4954,10 +4954,10 @@
         <v>201</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E113" s="22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include PSSM specific requirements.
Change-Id: I7c2212416836f1a87b54f069543ceb98ee6cbb28
Signed-off-by: jeremie.tatibouet <jeremie.tatibouet@cea.fr>
</commit_message>
<xml_diff>
--- a/Documents/PSSM-Requirements.xlsx
+++ b/Documents/PSSM-Requirements.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="367">
   <si>
     <t>Event_001</t>
   </si>
@@ -871,9 +871,6 @@
     <t>When an event is dispatched, that event can only initiate a RTC step if the transition(s) it enables materialize a valid path to a new state machine configuration. If this event only enable transition(s) that cannot bring the state machine to a valid configuration then this event is lost.</t>
   </si>
   <si>
-    <t>Deferred 005 Test verifies this requirement</t>
-  </si>
-  <si>
     <t>Deferred_004</t>
   </si>
   <si>
@@ -886,55 +883,25 @@
     <t>Deferred_006</t>
   </si>
   <si>
-    <t>Deferred 006 - A Test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Deferred 006 - B Test verifies this requirement</t>
-  </si>
-  <si>
     <t>A state is not allowed to defer an event occurrence for which a doActivity invoked from that state has already registered an event accepter. As an example, if S is dispatched and a state S1 can defer that event occurrence then S can only be deferred if S1 has not invoked a doActivity which has registered an event accepter for S.</t>
   </si>
   <si>
-    <t>A doActivity is allowed to accept directly from the deferred pool of the state machine an event occurrence deferred by the state from which it was invoked and for wich it is registering an event accepter. As an example, if S has been deferred by state S1 and the doActivity invoked from S1 registers an event accepter for S then S is accepted by the doActivity from the deferred event pool.</t>
-  </si>
-  <si>
     <t>A specialized StateMachine will have all the elements of the general StateMachine, and it may include additional elements. Regions may be added. Inherited Regions may be redefined by extension: States and Vertices are inherited, and States and Transitions of the Regions of the StateMachine may be redefined.</t>
   </si>
   <si>
-    <t>Redefinition001_Test, Redefinition002_Test and Redefinition003_Test verifies this requirement</t>
-  </si>
-  <si>
     <t>A state can have entry, doActivity and exit behaviors. If the redefining state does not declare one of these behavior then this behavior if specified in the redefined state (direct or indirect) is inherited by the redefining state.</t>
   </si>
   <si>
     <t>The set of deferrable trigger of a redefining state is the set of deferrable triggers declared by that state plus the set of deferrable triggers declared in redefined (directcly or indirectly) states.</t>
   </si>
   <si>
-    <t>The set of trigger owned by a redefining transition is the set of trigger delcared by that transition plus the set of trigger defined in redefined (directly or indirectly) transition.</t>
-  </si>
-  <si>
     <t>A transition can have an effect behavior. If a redefining transition does not declare an effect behavior then if a redefined (direct or indirect) transition declares an effect, this latter is inherited by the redefining transition.</t>
   </si>
   <si>
-    <t>Redefinition006_Test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Redefinition004_Test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Redefinition005_Test verifies this requirement</t>
-  </si>
-  <si>
-    <t>Redefinition002_Test verifies this requirement</t>
-  </si>
-  <si>
     <t xml:space="preserve">A transition can have an effect behavior. If a redefining transition declares an effect behavior, then this behavior is used (i.e. it replaces if any an effect specified by a redefined transition). </t>
   </si>
   <si>
     <t>A state can have entry, doActivity and exit behaviors. If the redefining state has one of this behavior then this latter is used (i.e. it replaces if any the behavior that may have been specified by a redefined state)</t>
-  </si>
-  <si>
-    <t>Redefinition003_Test verifies this requirement</t>
   </si>
   <si>
     <t>Redefinition_002</t>
@@ -1722,6 +1689,85 @@
 Fork 001.
 Fork 002.
 Entering 010.</t>
+  </si>
+  <si>
+    <t>Redefinition001.
+Note that also Redefinition 002 and Redefinition003 verify this requirement.</t>
+  </si>
+  <si>
+    <t>No dedicated test.
+Nevertheless support for this requirement is shown in Entry 002 E and Junction 004.</t>
+  </si>
+  <si>
+    <t>This is clearly related to Transition 024. We definitely need a test for that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dedicated test.
+Nevertheless support for this requirement is shown Junction 004 and Junction 005. </t>
+  </si>
+  <si>
+    <t>No dedicated test. 
+Nevertheless support for this requirement is shown in Junction 006, and Event 017 B.</t>
+  </si>
+  <si>
+    <t>No dedicated test.
+Nevertheless support for this requirement is shown in Event 019 A, Event 019 B and Event 019 C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dedicated test.
+Nevertheless support for this requirement is shown in Event 019 D, </t>
+  </si>
+  <si>
+    <t>No dedicated test.
+Nevertheless support for this requirement is shown in Event 019 E.</t>
+  </si>
+  <si>
+    <t>Deferred 005.</t>
+  </si>
+  <si>
+    <t>A doActivity is allowed to accept directly from the deferred pool of the state machine an event occurrence deferred by the state from which it was invoked and for which it is registering an event accepter. As an example, if S has been deferred by state S1 and the doActivity invoked from S1 registers an event accepter for S then S is accepted by the doActivity from the deferred event pool.</t>
+  </si>
+  <si>
+    <t>The set of trigger owned by a redefining transition is the set of trigger declared by that transition plus the set of trigger defined in redefined (directly or indirectly) transition.</t>
+  </si>
+  <si>
+    <t>Redefinition004.</t>
+  </si>
+  <si>
+    <t>Deferred 006 A.</t>
+  </si>
+  <si>
+    <t>Deferred 006 B.</t>
+  </si>
+  <si>
+    <t>Redefinition 002.</t>
+  </si>
+  <si>
+    <t>Redefinition 005.</t>
+  </si>
+  <si>
+    <t>Redefinition 006.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Redefinition 004.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Redefinition 005 must be improved to account for effect overriding.</t>
+    </r>
+  </si>
+  <si>
+    <t>Redefinition 001. 
+Redefinition 002.
+Redefinition 003.</t>
   </si>
 </sst>
 </file>
@@ -4359,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4442,10 +4488,10 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>196</v>
@@ -4454,7 +4500,7 @@
         <v>197</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -4474,7 +4520,7 @@
         <v>198</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -4494,7 +4540,7 @@
         <v>198</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -4514,7 +4560,7 @@
         <v>198</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -4534,7 +4580,7 @@
         <v>198</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -4554,7 +4600,7 @@
         <v>198</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -4574,7 +4620,7 @@
         <v>198</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
@@ -4594,7 +4640,7 @@
         <v>198</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -4614,7 +4660,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -4634,7 +4680,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -4654,7 +4700,7 @@
         <v>198</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -4674,7 +4720,7 @@
         <v>198</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -4694,7 +4740,7 @@
         <v>198</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -4714,7 +4760,7 @@
         <v>198</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -4734,7 +4780,7 @@
         <v>198</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -4754,7 +4800,7 @@
         <v>198</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -4774,7 +4820,7 @@
         <v>198</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
@@ -4794,7 +4840,7 @@
         <v>198</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
@@ -4814,7 +4860,7 @@
         <v>198</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -4834,7 +4880,7 @@
         <v>198</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
@@ -4854,7 +4900,7 @@
         <v>198</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -4894,7 +4940,7 @@
         <v>198</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -4934,7 +4980,7 @@
         <v>198</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -4954,7 +5000,7 @@
         <v>198</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
@@ -4974,7 +5020,7 @@
         <v>198</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
@@ -5034,7 +5080,7 @@
         <v>198</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -5054,7 +5100,7 @@
         <v>198</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
@@ -5094,7 +5140,7 @@
         <v>198</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -5114,7 +5160,7 @@
         <v>198</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
@@ -5134,7 +5180,7 @@
         <v>198</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -5154,7 +5200,7 @@
         <v>198</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
@@ -5174,7 +5220,7 @@
         <v>198</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
@@ -5234,7 +5280,7 @@
         <v>198</v>
       </c>
       <c r="E45" s="41" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
@@ -5254,7 +5300,7 @@
         <v>198</v>
       </c>
       <c r="E46" s="41" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
@@ -5274,7 +5320,7 @@
         <v>198</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
@@ -5294,7 +5340,7 @@
         <v>198</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
@@ -5314,7 +5360,7 @@
         <v>198</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
@@ -5334,7 +5380,7 @@
         <v>198</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -5354,7 +5400,7 @@
         <v>198</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
@@ -5374,7 +5420,7 @@
         <v>198</v>
       </c>
       <c r="E52" s="41" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
@@ -5414,7 +5460,7 @@
         <v>198</v>
       </c>
       <c r="E54" s="41" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -5434,7 +5480,7 @@
         <v>198</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -5474,7 +5520,7 @@
         <v>198</v>
       </c>
       <c r="E57" s="41" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
@@ -5494,7 +5540,7 @@
         <v>198</v>
       </c>
       <c r="E58" s="41" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
@@ -5514,7 +5560,7 @@
         <v>198</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
@@ -5534,7 +5580,7 @@
         <v>198</v>
       </c>
       <c r="E60" s="41" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
@@ -5554,7 +5600,7 @@
         <v>198</v>
       </c>
       <c r="E61" s="41" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
@@ -5574,7 +5620,7 @@
         <v>198</v>
       </c>
       <c r="E62" s="41" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
@@ -5614,7 +5660,7 @@
         <v>198</v>
       </c>
       <c r="E64" s="41" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
@@ -5634,7 +5680,7 @@
         <v>198</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="F65" s="18"/>
       <c r="G65" s="18"/>
@@ -5654,7 +5700,7 @@
         <v>198</v>
       </c>
       <c r="E66" s="41" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
@@ -5674,7 +5720,7 @@
         <v>198</v>
       </c>
       <c r="E67" s="41" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
@@ -5694,7 +5740,7 @@
         <v>198</v>
       </c>
       <c r="E68" s="41" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -5705,7 +5751,7 @@
         <v>88</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>198</v>
@@ -5714,7 +5760,7 @@
         <v>198</v>
       </c>
       <c r="E69" s="41" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
@@ -5734,7 +5780,7 @@
         <v>198</v>
       </c>
       <c r="E70" s="41" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
@@ -5754,7 +5800,7 @@
         <v>198</v>
       </c>
       <c r="E71" s="41" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="F71" s="18"/>
       <c r="G71" s="18"/>
@@ -5774,7 +5820,7 @@
         <v>198</v>
       </c>
       <c r="E72" s="41" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="F72" s="18"/>
       <c r="G72" s="18"/>
@@ -5794,7 +5840,7 @@
         <v>198</v>
       </c>
       <c r="E73" s="41" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="F73" s="18"/>
       <c r="G73" s="18"/>
@@ -5802,10 +5848,10 @@
     </row>
     <row r="74" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>198</v>
@@ -5814,7 +5860,7 @@
         <v>198</v>
       </c>
       <c r="E74" s="41" t="s">
-        <v>251</v>
+        <v>348</v>
       </c>
       <c r="F74" s="18"/>
       <c r="G74" s="18"/>
@@ -5822,10 +5868,10 @@
     </row>
     <row r="75" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="23" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>198</v>
@@ -5834,7 +5880,7 @@
         <v>198</v>
       </c>
       <c r="E75" s="41" t="s">
-        <v>251</v>
+        <v>366</v>
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
@@ -5854,7 +5900,7 @@
         <v>198</v>
       </c>
       <c r="E76" s="43" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
@@ -5874,7 +5920,7 @@
         <v>198</v>
       </c>
       <c r="E77" s="43" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
@@ -5894,7 +5940,7 @@
         <v>198</v>
       </c>
       <c r="E78" s="43" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
@@ -6074,7 +6120,7 @@
         <v>198</v>
       </c>
       <c r="E87" s="43" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="F87" s="18"/>
       <c r="G87" s="18"/>
@@ -6094,7 +6140,7 @@
         <v>198</v>
       </c>
       <c r="E88" s="43" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="F88" s="18"/>
       <c r="G88" s="18"/>
@@ -6114,7 +6160,7 @@
         <v>198</v>
       </c>
       <c r="E89" s="43" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F89" s="18"/>
       <c r="G89" s="18"/>
@@ -6154,7 +6200,7 @@
         <v>198</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="F91" s="18"/>
       <c r="G91" s="18"/>
@@ -6234,7 +6280,7 @@
         <v>198</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="F95" s="18"/>
       <c r="G95" s="18"/>
@@ -6254,7 +6300,7 @@
         <v>198</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F96" s="18"/>
       <c r="G96" s="18"/>
@@ -6274,7 +6320,7 @@
         <v>198</v>
       </c>
       <c r="E97" s="41" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
@@ -6294,7 +6340,7 @@
         <v>198</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="F98" s="18"/>
       <c r="G98" s="18"/>
@@ -6314,7 +6360,7 @@
         <v>198</v>
       </c>
       <c r="E99" s="41" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="F99" s="18"/>
       <c r="G99" s="18"/>
@@ -6334,7 +6380,7 @@
         <v>198</v>
       </c>
       <c r="E100" s="41" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F100" s="18"/>
       <c r="G100" s="18"/>
@@ -6354,7 +6400,7 @@
         <v>198</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="F101" s="18"/>
       <c r="G101" s="18"/>
@@ -6374,7 +6420,7 @@
         <v>198</v>
       </c>
       <c r="E102" s="48" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="F102" s="18"/>
       <c r="G102" s="18"/>
@@ -6394,7 +6440,7 @@
         <v>198</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
@@ -6414,7 +6460,7 @@
         <v>198</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="F104" s="18"/>
       <c r="G104" s="18"/>
@@ -6434,7 +6480,7 @@
         <v>198</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="F105" s="18"/>
       <c r="G105" s="18"/>
@@ -6474,7 +6520,7 @@
         <v>198</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F107" s="18"/>
       <c r="G107" s="18"/>
@@ -6494,7 +6540,7 @@
         <v>198</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F108" s="18"/>
       <c r="G108" s="18"/>
@@ -6514,7 +6560,7 @@
         <v>198</v>
       </c>
       <c r="E109" s="49" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F109" s="18"/>
       <c r="G109" s="18"/>
@@ -6534,7 +6580,7 @@
         <v>198</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F110" s="18"/>
       <c r="G110" s="18"/>
@@ -6554,7 +6600,7 @@
         <v>198</v>
       </c>
       <c r="E111" s="43" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="F111" s="18"/>
       <c r="G111" s="18"/>
@@ -6571,10 +6617,10 @@
         <v>198</v>
       </c>
       <c r="D112" s="17" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -6594,7 +6640,7 @@
         <v>198</v>
       </c>
       <c r="E113" s="43" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F113" s="18"/>
       <c r="G113" s="18"/>
@@ -6614,7 +6660,7 @@
         <v>198</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F114" s="18"/>
       <c r="G114" s="18"/>
@@ -6634,7 +6680,7 @@
         <v>198</v>
       </c>
       <c r="E115" s="43" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="F115" s="18"/>
       <c r="G115" s="18"/>
@@ -6665,7 +6711,9 @@
       <c r="D117" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E117" s="50"/>
+      <c r="E117" s="50" t="s">
+        <v>351</v>
+      </c>
       <c r="F117" s="18"/>
       <c r="G117" s="18"/>
       <c r="H117" s="18"/>
@@ -6683,7 +6731,9 @@
       <c r="D118" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E118" s="43"/>
+      <c r="E118" s="43" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="119" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="31" t="s">
@@ -6696,9 +6746,11 @@
         <v>198</v>
       </c>
       <c r="D119" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="E119" s="50"/>
+        <v>291</v>
+      </c>
+      <c r="E119" s="50" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="120" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
@@ -6713,7 +6765,9 @@
       <c r="D120" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E120" s="43"/>
+      <c r="E120" s="43" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="121" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="31" t="s">
@@ -6728,7 +6782,9 @@
       <c r="D121" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E121" s="50"/>
+      <c r="E121" s="50" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="122" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
@@ -6743,7 +6799,9 @@
       <c r="D122" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E122" s="43"/>
+      <c r="E122" s="43" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="123" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="31" t="s">
@@ -6758,15 +6816,17 @@
       <c r="D123" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E123" s="50"/>
+      <c r="E123" s="50" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="124" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="B124" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="B124" s="30" t="s">
-        <v>243</v>
-      </c>
       <c r="C124" s="17" t="s">
         <v>198</v>
       </c>
@@ -6774,15 +6834,15 @@
         <v>198</v>
       </c>
       <c r="E124" s="43" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B125" s="35" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C125" s="17" t="s">
         <v>198</v>
@@ -6791,15 +6851,15 @@
         <v>198</v>
       </c>
       <c r="E125" s="43" t="s">
-        <v>246</v>
+        <v>360</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>249</v>
+        <v>357</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>198</v>
@@ -6808,15 +6868,15 @@
         <v>198</v>
       </c>
       <c r="E126" s="43" t="s">
-        <v>247</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="34" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B127" s="35" t="s">
-        <v>254</v>
+        <v>358</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>198</v>
@@ -6825,15 +6885,15 @@
         <v>198</v>
       </c>
       <c r="E127" s="43" t="s">
-        <v>257</v>
+        <v>359</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>198</v>
@@ -6842,15 +6902,15 @@
         <v>198</v>
       </c>
       <c r="E128" s="43" t="s">
-        <v>262</v>
+        <v>365</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="34" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B129" s="35" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>198</v>
@@ -6859,15 +6919,15 @@
         <v>198</v>
       </c>
       <c r="E129" s="43" t="s">
-        <v>259</v>
+        <v>362</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C130" s="17" t="s">
         <v>198</v>
@@ -6876,15 +6936,15 @@
         <v>198</v>
       </c>
       <c r="E130" s="43" t="s">
-        <v>258</v>
+        <v>363</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="34" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B131" s="35" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C131" s="17" t="s">
         <v>198</v>
@@ -6893,15 +6953,15 @@
         <v>198</v>
       </c>
       <c r="E131" s="43" t="s">
-        <v>258</v>
+        <v>363</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C132" s="17" t="s">
         <v>198</v>
@@ -6910,7 +6970,7 @@
         <v>198</v>
       </c>
       <c r="E132" s="43" t="s">
-        <v>256</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Redefinition schemes and test descriptions. In addition terminate 002 test description is simplified and corrected.
Change-Id: Ia2fe80101d307b32e96c66cbdb1a0f78674e08f0
Signed-off-by: jeremie.tatibouet <jeremie.tatibouet@cea.fr>
</commit_message>
<xml_diff>
--- a/Documents/PSSM-Requirements.xlsx
+++ b/Documents/PSSM-Requirements.xlsx
@@ -687,9 +687,6 @@
     <t>it is possible for multiple mutually exclusive Transitions in a given Region to be enabled for firing by the same Event occurrence. In those cases, only one is selected and executed. Which of the enabled Transitions is chosen is determined by the Transition selection algorithm described below. (p.330)</t>
   </si>
   <si>
-    <t>There is no test to demonstrate such support for transitions chained in a compound transition.</t>
-  </si>
-  <si>
     <t>Duplication of Entering001</t>
   </si>
   <si>
@@ -1250,23 +1247,6 @@
 TransitionSelectionAlgorithm.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Behavior 003 A.
-Behavior 003 B.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note: for the moment no test shows concurrency with behaviors placed on substates.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">No dedicated test.
 Nevertheless History 002 A shows support for this requirement. </t>
   </si>
@@ -1767,6 +1747,13 @@
   <si>
     <t xml:space="preserve">No dedicated test
 Choice 005 demonstrates that guards evaluation for transitions outgoing a choice pseudostate occur during the step and not prior to that step. </t>
+  </si>
+  <si>
+    <t>Event 016 A demonstrates this for transitions which are not compound. Neverheless a dedicated test is required.</t>
+  </si>
+  <si>
+    <t>Behavior 003 A.
+Behavior 003 B.</t>
   </si>
 </sst>
 </file>
@@ -2650,9 +2637,6 @@
     <xf numFmtId="0" fontId="20" fillId="39" borderId="12" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2673,6 +2657,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="12" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -4404,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4487,10 +4474,10 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>264</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>265</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>196</v>
@@ -4498,8 +4485,8 @@
       <c r="D6" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="51" t="s">
-        <v>271</v>
+      <c r="E6" s="50" t="s">
+        <v>270</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -4519,7 +4506,7 @@
         <v>198</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -4539,7 +4526,7 @@
         <v>198</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -4559,7 +4546,7 @@
         <v>198</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -4579,7 +4566,7 @@
         <v>198</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -4599,7 +4586,7 @@
         <v>198</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -4619,7 +4606,7 @@
         <v>198</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
@@ -4639,7 +4626,7 @@
         <v>198</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -4659,7 +4646,7 @@
         <v>212</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -4679,7 +4666,7 @@
         <v>212</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -4699,7 +4686,7 @@
         <v>198</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -4719,7 +4706,7 @@
         <v>198</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -4739,7 +4726,7 @@
         <v>198</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -4759,7 +4746,7 @@
         <v>198</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -4779,7 +4766,7 @@
         <v>198</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -4799,7 +4786,7 @@
         <v>198</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -4819,7 +4806,7 @@
         <v>198</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
@@ -4839,7 +4826,7 @@
         <v>198</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>307</v>
+        <v>365</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
@@ -4859,7 +4846,7 @@
         <v>198</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -4879,7 +4866,7 @@
         <v>198</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
@@ -4899,7 +4886,7 @@
         <v>198</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -4918,8 +4905,8 @@
       <c r="D27" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E27" s="52" t="s">
-        <v>222</v>
+      <c r="E27" s="51" t="s">
+        <v>221</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
@@ -4930,7 +4917,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>198</v>
@@ -4939,7 +4926,7 @@
         <v>198</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -4958,8 +4945,8 @@
       <c r="D29" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E29" s="52" t="s">
-        <v>222</v>
+      <c r="E29" s="51" t="s">
+        <v>221</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
@@ -4979,7 +4966,7 @@
         <v>198</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -4999,7 +4986,7 @@
         <v>198</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
@@ -5019,7 +5006,7 @@
         <v>198</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
@@ -5079,7 +5066,7 @@
         <v>198</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -5099,7 +5086,7 @@
         <v>198</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
@@ -5139,7 +5126,7 @@
         <v>198</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -5159,7 +5146,7 @@
         <v>198</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
@@ -5179,7 +5166,7 @@
         <v>198</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -5199,7 +5186,7 @@
         <v>198</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
@@ -5219,7 +5206,7 @@
         <v>198</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
@@ -5238,7 +5225,7 @@
       <c r="D43" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="51" t="s">
         <v>219</v>
       </c>
       <c r="F43" s="18"/>
@@ -5258,8 +5245,8 @@
       <c r="D44" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E44" s="52" t="s">
-        <v>223</v>
+      <c r="E44" s="51" t="s">
+        <v>222</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
@@ -5270,7 +5257,7 @@
         <v>178</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>198</v>
@@ -5279,7 +5266,7 @@
         <v>198</v>
       </c>
       <c r="E45" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
@@ -5299,7 +5286,7 @@
         <v>198</v>
       </c>
       <c r="E46" s="41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
@@ -5319,7 +5306,7 @@
         <v>198</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
@@ -5339,7 +5326,7 @@
         <v>198</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
@@ -5359,7 +5346,7 @@
         <v>198</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
@@ -5379,7 +5366,7 @@
         <v>198</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -5399,7 +5386,7 @@
         <v>198</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
@@ -5419,7 +5406,7 @@
         <v>198</v>
       </c>
       <c r="E52" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
@@ -5438,8 +5425,8 @@
       <c r="D53" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="45" t="s">
-        <v>221</v>
+      <c r="E53" s="52" t="s">
+        <v>364</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
@@ -5459,7 +5446,7 @@
         <v>198</v>
       </c>
       <c r="E54" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -5479,7 +5466,7 @@
         <v>198</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -5519,7 +5506,7 @@
         <v>198</v>
       </c>
       <c r="E57" s="41" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
@@ -5539,7 +5526,7 @@
         <v>198</v>
       </c>
       <c r="E58" s="41" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
@@ -5559,7 +5546,7 @@
         <v>198</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
@@ -5579,7 +5566,7 @@
         <v>198</v>
       </c>
       <c r="E60" s="41" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
@@ -5599,7 +5586,7 @@
         <v>198</v>
       </c>
       <c r="E61" s="41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
@@ -5619,7 +5606,7 @@
         <v>198</v>
       </c>
       <c r="E62" s="41" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
@@ -5659,7 +5646,7 @@
         <v>198</v>
       </c>
       <c r="E64" s="41" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
@@ -5679,7 +5666,7 @@
         <v>198</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F65" s="18"/>
       <c r="G65" s="18"/>
@@ -5699,7 +5686,7 @@
         <v>198</v>
       </c>
       <c r="E66" s="41" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
@@ -5719,7 +5706,7 @@
         <v>198</v>
       </c>
       <c r="E67" s="41" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
@@ -5739,7 +5726,7 @@
         <v>198</v>
       </c>
       <c r="E68" s="41" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -5750,7 +5737,7 @@
         <v>88</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>198</v>
@@ -5759,7 +5746,7 @@
         <v>198</v>
       </c>
       <c r="E69" s="41" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
@@ -5779,7 +5766,7 @@
         <v>198</v>
       </c>
       <c r="E70" s="41" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
@@ -5799,7 +5786,7 @@
         <v>198</v>
       </c>
       <c r="E71" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F71" s="18"/>
       <c r="G71" s="18"/>
@@ -5819,7 +5806,7 @@
         <v>198</v>
       </c>
       <c r="E72" s="41" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F72" s="18"/>
       <c r="G72" s="18"/>
@@ -5839,7 +5826,7 @@
         <v>198</v>
       </c>
       <c r="E73" s="41" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F73" s="18"/>
       <c r="G73" s="18"/>
@@ -5847,10 +5834,10 @@
     </row>
     <row r="74" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>198</v>
@@ -5859,7 +5846,7 @@
         <v>198</v>
       </c>
       <c r="E74" s="41" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F74" s="18"/>
       <c r="G74" s="18"/>
@@ -5867,10 +5854,10 @@
     </row>
     <row r="75" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>198</v>
@@ -5879,7 +5866,7 @@
         <v>198</v>
       </c>
       <c r="E75" s="41" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
@@ -5899,7 +5886,7 @@
         <v>198</v>
       </c>
       <c r="E76" s="43" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
@@ -5919,7 +5906,7 @@
         <v>198</v>
       </c>
       <c r="E77" s="43" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
@@ -5939,7 +5926,7 @@
         <v>198</v>
       </c>
       <c r="E78" s="43" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
@@ -6058,7 +6045,7 @@
       <c r="D84" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E84" s="46" t="s">
+      <c r="E84" s="45" t="s">
         <v>205</v>
       </c>
       <c r="F84" s="18"/>
@@ -6078,7 +6065,7 @@
       <c r="D85" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E85" s="46" t="s">
+      <c r="E85" s="45" t="s">
         <v>205</v>
       </c>
       <c r="F85" s="18"/>
@@ -6098,7 +6085,7 @@
       <c r="D86" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E86" s="46" t="s">
+      <c r="E86" s="45" t="s">
         <v>205</v>
       </c>
       <c r="F86" s="18"/>
@@ -6119,7 +6106,7 @@
         <v>198</v>
       </c>
       <c r="E87" s="43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F87" s="18"/>
       <c r="G87" s="18"/>
@@ -6139,7 +6126,7 @@
         <v>198</v>
       </c>
       <c r="E88" s="43" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F88" s="18"/>
       <c r="G88" s="18"/>
@@ -6159,7 +6146,7 @@
         <v>198</v>
       </c>
       <c r="E89" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F89" s="18"/>
       <c r="G89" s="18"/>
@@ -6178,7 +6165,7 @@
       <c r="D90" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E90" s="47" t="s">
+      <c r="E90" s="46" t="s">
         <v>206</v>
       </c>
       <c r="F90" s="18"/>
@@ -6199,7 +6186,7 @@
         <v>198</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F91" s="18"/>
       <c r="G91" s="18"/>
@@ -6279,7 +6266,7 @@
         <v>198</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F95" s="18"/>
       <c r="G95" s="18"/>
@@ -6299,7 +6286,7 @@
         <v>198</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F96" s="18"/>
       <c r="G96" s="18"/>
@@ -6319,7 +6306,7 @@
         <v>198</v>
       </c>
       <c r="E97" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
@@ -6339,7 +6326,7 @@
         <v>198</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F98" s="18"/>
       <c r="G98" s="18"/>
@@ -6359,7 +6346,7 @@
         <v>198</v>
       </c>
       <c r="E99" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F99" s="18"/>
       <c r="G99" s="18"/>
@@ -6379,7 +6366,7 @@
         <v>198</v>
       </c>
       <c r="E100" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F100" s="18"/>
       <c r="G100" s="18"/>
@@ -6399,7 +6386,7 @@
         <v>198</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F101" s="18"/>
       <c r="G101" s="18"/>
@@ -6418,8 +6405,8 @@
       <c r="D102" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E102" s="48" t="s">
-        <v>282</v>
+      <c r="E102" s="47" t="s">
+        <v>281</v>
       </c>
       <c r="F102" s="18"/>
       <c r="G102" s="18"/>
@@ -6439,7 +6426,7 @@
         <v>198</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
@@ -6459,7 +6446,7 @@
         <v>198</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F104" s="18"/>
       <c r="G104" s="18"/>
@@ -6479,7 +6466,7 @@
         <v>198</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F105" s="18"/>
       <c r="G105" s="18"/>
@@ -6519,7 +6506,7 @@
         <v>198</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F107" s="18"/>
       <c r="G107" s="18"/>
@@ -6539,7 +6526,7 @@
         <v>198</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F108" s="18"/>
       <c r="G108" s="18"/>
@@ -6558,8 +6545,8 @@
       <c r="D109" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E109" s="49" t="s">
-        <v>287</v>
+      <c r="E109" s="48" t="s">
+        <v>286</v>
       </c>
       <c r="F109" s="18"/>
       <c r="G109" s="18"/>
@@ -6579,7 +6566,7 @@
         <v>198</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F110" s="18"/>
       <c r="G110" s="18"/>
@@ -6599,7 +6586,7 @@
         <v>198</v>
       </c>
       <c r="E111" s="43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F111" s="18"/>
       <c r="G111" s="18"/>
@@ -6619,7 +6606,7 @@
         <v>198</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -6639,7 +6626,7 @@
         <v>198</v>
       </c>
       <c r="E113" s="43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F113" s="18"/>
       <c r="G113" s="18"/>
@@ -6659,7 +6646,7 @@
         <v>198</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F114" s="18"/>
       <c r="G114" s="18"/>
@@ -6679,7 +6666,7 @@
         <v>198</v>
       </c>
       <c r="E115" s="43" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F115" s="18"/>
       <c r="G115" s="18"/>
@@ -6687,7 +6674,7 @@
     </row>
     <row r="116" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B116" s="37"/>
       <c r="C116" s="37"/>
@@ -6699,10 +6686,10 @@
     </row>
     <row r="117" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B117" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C117" s="33" t="s">
         <v>198</v>
@@ -6710,8 +6697,8 @@
       <c r="D117" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E117" s="50" t="s">
-        <v>348</v>
+      <c r="E117" s="49" t="s">
+        <v>346</v>
       </c>
       <c r="F117" s="18"/>
       <c r="G117" s="18"/>
@@ -6719,10 +6706,10 @@
     </row>
     <row r="118" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C118" s="17" t="s">
         <v>198</v>
@@ -6731,32 +6718,32 @@
         <v>198</v>
       </c>
       <c r="E118" s="43" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="B119" s="32" t="s">
-        <v>229</v>
-      </c>
       <c r="C119" s="33" t="s">
         <v>198</v>
       </c>
       <c r="D119" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E119" s="50" t="s">
-        <v>365</v>
+      <c r="E119" s="49" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>198</v>
@@ -6765,15 +6752,15 @@
         <v>198</v>
       </c>
       <c r="E120" s="43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B121" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C121" s="33" t="s">
         <v>198</v>
@@ -6781,16 +6768,16 @@
       <c r="D121" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E121" s="50" t="s">
-        <v>350</v>
+      <c r="E121" s="49" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C122" s="17" t="s">
         <v>198</v>
@@ -6799,33 +6786,33 @@
         <v>198</v>
       </c>
       <c r="E122" s="43" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="B123" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="B123" s="32" t="s">
-        <v>238</v>
-      </c>
       <c r="C123" s="33" t="s">
         <v>198</v>
       </c>
       <c r="D123" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E123" s="50" t="s">
-        <v>352</v>
+      <c r="E123" s="49" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B124" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="B124" s="30" t="s">
-        <v>242</v>
-      </c>
       <c r="C124" s="17" t="s">
         <v>198</v>
       </c>
@@ -6833,15 +6820,15 @@
         <v>198</v>
       </c>
       <c r="E124" s="43" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B125" s="35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C125" s="17" t="s">
         <v>198</v>
@@ -6850,15 +6837,15 @@
         <v>198</v>
       </c>
       <c r="E125" s="43" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>198</v>
@@ -6867,15 +6854,15 @@
         <v>198</v>
       </c>
       <c r="E126" s="43" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B127" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>198</v>
@@ -6884,15 +6871,15 @@
         <v>198</v>
       </c>
       <c r="E127" s="43" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>198</v>
@@ -6901,15 +6888,15 @@
         <v>198</v>
       </c>
       <c r="E128" s="43" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B129" s="35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>198</v>
@@ -6918,15 +6905,15 @@
         <v>198</v>
       </c>
       <c r="E129" s="43" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C130" s="17" t="s">
         <v>198</v>
@@ -6935,15 +6922,15 @@
         <v>198</v>
       </c>
       <c r="E130" s="43" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B131" s="35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C131" s="17" t="s">
         <v>198</v>
@@ -6952,15 +6939,15 @@
         <v>198</v>
       </c>
       <c r="E131" s="43" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C132" s="17" t="s">
         <v>198</v>
@@ -6969,7 +6956,7 @@
         <v>198</v>
       </c>
       <c r="E132" s="43" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>